<commit_message>
✨feat(auth): Implement user request and response DTOs for registration, login, and updates
Author: Zheyun Zhao <jp2022213670@qmul.ac.uk>
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
✨ feat(client): Update alert label color for better visibility
Author: Yujie Yang <jp2022213663@qmul.ac.uk>
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat(client): Complete signup design
Completed signup and login design (only UI design)

Author: Youhao Zhong <jp2022213676@qmul.ac.uk>
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat(client): Implement Login and Signup
The front-end and back-end integration for login and registration has been completed, and now accounts can be registered and logged in

Author: Youhao Zhong <jp2022213676@qmul.ac.uk>
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
:sparkles: Add a new test for new method GetTransactionsByAccountId
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
✨feat(ai): Add AI messaging functionality with user interaction and dynamic content loading
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
🐛fix(env): Add environment configuration and update jsonStorage location
Author: Zheyun Zhao <jp2022213670@qmul.ac.uk>
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
✨feat(server): Implement account management features including add, delete, and retrieve accounts.
Author: Zheyun Zhao <jp2022213670@qmul.ac.uk>
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat(server): Add Dashboard Handler to process request of dashboard
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
:sparkles: (client): user info management
All content pane have update a userInfo field to get user's information.

Author: Youhao Zhong <jp2022213676@qmul.ac.uk>
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -203,17 +203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.71484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.40234375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.421875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.0703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.61328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.24609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.01953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.98046875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.25390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.44140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="16.640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.87890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
✨ feat(server): Add transaction csv and excel export function
</commit_message>
<xml_diff>
--- a/aiconomy-server/src/test/resources/transactions.xlsx
+++ b/aiconomy-server/src/test/resources/transactions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -44,6 +44,12 @@
     <t>merchantOrderId</t>
   </si>
   <si>
+    <t>accountId</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
     <t>remark</t>
   </si>
   <si>
@@ -77,6 +83,12 @@
     <t>7890</t>
   </si>
   <si>
+    <t>acc1</t>
+  </si>
+  <si>
+    <t>AureliaSKY</t>
+  </si>
+  <si>
     <t>购买iPhone 15</t>
   </si>
   <si>
@@ -105,6 +117,9 @@
   </si>
   <si>
     <t>7891</t>
+  </si>
+  <si>
+    <t>acc2</t>
   </si>
   <si>
     <t>收到MacBook款项</t>
@@ -197,7 +212,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -213,7 +228,9 @@
     <col min="8" max="8" width="15.4296875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="6.54296875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="16.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="10.6171875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="16.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -250,145 +267,175 @@
       <c r="K1" t="s" s="0">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="0">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>31</v>
+      <c r="M3" t="s" s="0">
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>39</v>
+        <v>23</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s" s="0">
-        <v>46</v>
+      <c r="M5" t="s" s="0">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>